<commit_message>
Finish Selec and on process merge
</commit_message>
<xml_diff>
--- a/docs/Checklist-withFormula.xlsx
+++ b/docs/Checklist-withFormula.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sinhvien\Session3\CTDL_GT\BTTH\Lab3\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C6A754A5-1609-45AF-BA16-D558A392465D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C31EF711-89B0-4FBA-B045-E4943205C40C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{8CE66FDF-E979-4E9F-A8C3-831D61C41828}"/>
   </bookViews>
@@ -342,18 +342,36 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -363,24 +381,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -757,7 +757,7 @@
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="73" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -774,24 +774,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="19" t="s">
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="H1" s="16"/>
+      <c r="H1" s="25"/>
     </row>
     <row r="2" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="20"/>
+      <c r="B2" s="26"/>
       <c r="C2" s="2" t="s">
         <v>0</v>
       </c>
@@ -801,7 +801,7 @@
       <c r="E2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="18"/>
+      <c r="F2" s="22"/>
       <c r="G2" s="6" t="s">
         <v>30</v>
       </c>
@@ -810,10 +810,10 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="15"/>
+      <c r="B3" s="19"/>
       <c r="C3" s="14">
         <v>21120504</v>
       </c>
@@ -823,7 +823,7 @@
       <c r="E3" s="14">
         <v>21120504</v>
       </c>
-      <c r="F3" s="18"/>
+      <c r="F3" s="22"/>
       <c r="G3" s="6" t="s">
         <v>31</v>
       </c>
@@ -832,10 +832,10 @@
       </c>
     </row>
     <row r="4" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="15"/>
+      <c r="B4" s="19"/>
       <c r="C4" s="14">
         <v>21120505</v>
       </c>
@@ -845,7 +845,7 @@
       <c r="E4" s="14">
         <v>21120505</v>
       </c>
-      <c r="F4" s="18"/>
+      <c r="F4" s="22"/>
       <c r="G4" s="6" t="s">
         <v>32</v>
       </c>
@@ -854,10 +854,10 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="15"/>
+      <c r="B5" s="19"/>
       <c r="C5" s="14">
         <v>21120521</v>
       </c>
@@ -867,7 +867,7 @@
       <c r="E5" s="14">
         <v>21120521</v>
       </c>
-      <c r="F5" s="18"/>
+      <c r="F5" s="22"/>
       <c r="G5" s="6" t="s">
         <v>33</v>
       </c>
@@ -876,10 +876,10 @@
       </c>
     </row>
     <row r="6" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="15"/>
+      <c r="A6" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="19"/>
       <c r="C6" s="14">
         <v>21120499</v>
       </c>
@@ -889,7 +889,7 @@
       <c r="E6" s="14">
         <v>21120499</v>
       </c>
-      <c r="F6" s="18"/>
+      <c r="F6" s="22"/>
       <c r="G6" s="6" t="s">
         <v>34</v>
       </c>
@@ -898,10 +898,10 @@
       </c>
     </row>
     <row r="7" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="15"/>
+      <c r="B7" s="19"/>
       <c r="C7" s="14">
         <v>21120504</v>
       </c>
@@ -911,15 +911,15 @@
       <c r="E7" s="14">
         <v>21120504</v>
       </c>
-      <c r="F7" s="18"/>
-      <c r="G7" s="21"/>
-      <c r="H7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="28"/>
     </row>
     <row r="8" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="15"/>
+      <c r="B8" s="19"/>
       <c r="C8" s="14">
         <v>21120505</v>
       </c>
@@ -929,17 +929,17 @@
       <c r="E8" s="14">
         <v>21120505</v>
       </c>
-      <c r="F8" s="18"/>
-      <c r="G8" s="19" t="s">
+      <c r="F8" s="22"/>
+      <c r="G8" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="H8" s="16"/>
+      <c r="H8" s="25"/>
     </row>
     <row r="9" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="15"/>
+      <c r="B9" s="19"/>
       <c r="C9" s="14">
         <v>21120521</v>
       </c>
@@ -949,7 +949,7 @@
       <c r="E9" s="14">
         <v>21120521</v>
       </c>
-      <c r="F9" s="18"/>
+      <c r="F9" s="22"/>
       <c r="G9" s="7" t="s">
         <v>14</v>
       </c>
@@ -958,10 +958,10 @@
       </c>
     </row>
     <row r="10" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="15"/>
+      <c r="B10" s="19"/>
       <c r="C10" s="14">
         <v>21120499</v>
       </c>
@@ -971,7 +971,7 @@
       <c r="E10" s="14">
         <v>21120499</v>
       </c>
-      <c r="F10" s="18"/>
+      <c r="F10" s="22"/>
       <c r="G10" s="7" t="s">
         <v>15</v>
       </c>
@@ -980,10 +980,10 @@
       </c>
     </row>
     <row r="11" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="15"/>
+      <c r="A11" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="19"/>
       <c r="C11" s="1">
         <v>21120504</v>
       </c>
@@ -993,7 +993,7 @@
       <c r="E11" s="1">
         <v>21120504</v>
       </c>
-      <c r="F11" s="18"/>
+      <c r="F11" s="22"/>
       <c r="G11" s="7" t="s">
         <v>25</v>
       </c>
@@ -1002,10 +1002,10 @@
       </c>
     </row>
     <row r="12" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="15" t="s">
+      <c r="A12" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="15"/>
+      <c r="B12" s="19"/>
       <c r="C12" s="1">
         <v>21120505</v>
       </c>
@@ -1015,7 +1015,7 @@
       <c r="E12" s="1">
         <v>21120505</v>
       </c>
-      <c r="F12" s="18"/>
+      <c r="F12" s="22"/>
       <c r="G12" s="7" t="s">
         <v>26</v>
       </c>
@@ -1024,10 +1024,10 @@
       </c>
     </row>
     <row r="13" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="15" t="s">
+      <c r="A13" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="15"/>
+      <c r="B13" s="19"/>
       <c r="C13" s="1">
         <v>21120521</v>
       </c>
@@ -1037,7 +1037,7 @@
       <c r="E13" s="1">
         <v>21120521</v>
       </c>
-      <c r="F13" s="18"/>
+      <c r="F13" s="22"/>
       <c r="G13" s="7" t="s">
         <v>27</v>
       </c>
@@ -1046,22 +1046,22 @@
       </c>
     </row>
     <row r="14" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="25"/>
-      <c r="B14" s="26"/>
-      <c r="C14" s="26"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="28"/>
+      <c r="A14" s="20"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="24"/>
     </row>
     <row r="15" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="17" t="s">
+      <c r="A15" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="24"/>
-      <c r="C15" s="24"/>
-      <c r="D15" s="19"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="18"/>
       <c r="E15" s="8"/>
       <c r="J15"/>
     </row>
@@ -1078,7 +1078,7 @@
       <c r="J16"/>
     </row>
     <row r="17" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="23" t="s">
+      <c r="A17" s="15" t="s">
         <v>0</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -1094,7 +1094,7 @@
       <c r="J17"/>
     </row>
     <row r="18" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="23"/>
+      <c r="A18" s="15"/>
       <c r="B18" s="1" t="s">
         <v>20</v>
       </c>
@@ -1108,7 +1108,7 @@
       <c r="J18"/>
     </row>
     <row r="19" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="23"/>
+      <c r="A19" s="15"/>
       <c r="B19" s="1" t="s">
         <v>23</v>
       </c>
@@ -1122,7 +1122,7 @@
       <c r="J19"/>
     </row>
     <row r="20" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="23"/>
+      <c r="A20" s="15"/>
       <c r="B20" s="1" t="s">
         <v>24</v>
       </c>
@@ -1136,7 +1136,7 @@
       <c r="J20"/>
     </row>
     <row r="21" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A21" s="23" t="s">
+      <c r="A21" s="15" t="s">
         <v>1</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -1152,7 +1152,7 @@
       <c r="J21"/>
     </row>
     <row r="22" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A22" s="23"/>
+      <c r="A22" s="15"/>
       <c r="B22" s="1" t="s">
         <v>20</v>
       </c>
@@ -1166,7 +1166,7 @@
       <c r="J22"/>
     </row>
     <row r="23" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A23" s="23"/>
+      <c r="A23" s="15"/>
       <c r="B23" s="1" t="s">
         <v>23</v>
       </c>
@@ -1180,7 +1180,7 @@
       <c r="J23"/>
     </row>
     <row r="24" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A24" s="23"/>
+      <c r="A24" s="15"/>
       <c r="B24" s="1" t="s">
         <v>24</v>
       </c>
@@ -1237,11 +1237,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="A21:A24"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="A17:A20"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:H14"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="F1:F13"/>
@@ -1258,6 +1253,11 @@
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A21:A24"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="A17:A20"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:H14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1283,24 +1283,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="19" t="s">
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="H1" s="16"/>
+      <c r="H1" s="25"/>
     </row>
     <row r="2" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="20"/>
+      <c r="B2" s="26"/>
       <c r="C2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1310,7 +1310,7 @@
       <c r="E2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="18"/>
+      <c r="F2" s="22"/>
       <c r="G2" s="6" t="s">
         <v>30</v>
       </c>
@@ -1319,10 +1319,10 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="15"/>
+      <c r="B3" s="19"/>
       <c r="C3" s="1">
         <v>5</v>
       </c>
@@ -1332,7 +1332,7 @@
       <c r="E3" s="1">
         <v>10</v>
       </c>
-      <c r="F3" s="18"/>
+      <c r="F3" s="22"/>
       <c r="G3" s="6" t="s">
         <v>31</v>
       </c>
@@ -1341,10 +1341,10 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="15"/>
+      <c r="B4" s="19"/>
       <c r="C4" s="1">
         <v>5</v>
       </c>
@@ -1354,7 +1354,7 @@
       <c r="E4" s="1">
         <v>10</v>
       </c>
-      <c r="F4" s="18"/>
+      <c r="F4" s="22"/>
       <c r="G4" s="6" t="s">
         <v>32</v>
       </c>
@@ -1363,10 +1363,10 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="15"/>
+      <c r="B5" s="19"/>
       <c r="C5" s="1">
         <v>5</v>
       </c>
@@ -1376,7 +1376,7 @@
       <c r="E5" s="1">
         <v>10</v>
       </c>
-      <c r="F5" s="18"/>
+      <c r="F5" s="22"/>
       <c r="G5" s="6" t="s">
         <v>33</v>
       </c>
@@ -1385,10 +1385,10 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="15"/>
+      <c r="A6" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="19"/>
       <c r="C6" s="1">
         <v>5</v>
       </c>
@@ -1398,7 +1398,7 @@
       <c r="E6" s="1">
         <v>10</v>
       </c>
-      <c r="F6" s="18"/>
+      <c r="F6" s="22"/>
       <c r="G6" s="6" t="s">
         <v>34</v>
       </c>
@@ -1407,10 +1407,10 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="15"/>
+      <c r="B7" s="19"/>
       <c r="C7" s="1">
         <v>5</v>
       </c>
@@ -1420,15 +1420,15 @@
       <c r="E7" s="1">
         <v>10</v>
       </c>
-      <c r="F7" s="18"/>
-      <c r="G7" s="21"/>
-      <c r="H7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="28"/>
     </row>
     <row r="8" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="15"/>
+      <c r="B8" s="19"/>
       <c r="C8" s="1">
         <v>5</v>
       </c>
@@ -1438,17 +1438,17 @@
       <c r="E8" s="1">
         <v>10</v>
       </c>
-      <c r="F8" s="18"/>
-      <c r="G8" s="19" t="s">
+      <c r="F8" s="22"/>
+      <c r="G8" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="H8" s="16"/>
+      <c r="H8" s="25"/>
     </row>
     <row r="9" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="15"/>
+      <c r="B9" s="19"/>
       <c r="C9" s="1">
         <v>5</v>
       </c>
@@ -1458,7 +1458,7 @@
       <c r="E9" s="1">
         <v>10</v>
       </c>
-      <c r="F9" s="18"/>
+      <c r="F9" s="22"/>
       <c r="G9" s="7" t="s">
         <v>14</v>
       </c>
@@ -1467,10 +1467,10 @@
       </c>
     </row>
     <row r="10" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="15"/>
+      <c r="B10" s="19"/>
       <c r="C10" s="1">
         <v>5</v>
       </c>
@@ -1480,7 +1480,7 @@
       <c r="E10" s="1">
         <v>10</v>
       </c>
-      <c r="F10" s="18"/>
+      <c r="F10" s="22"/>
       <c r="G10" s="7" t="s">
         <v>15</v>
       </c>
@@ -1489,10 +1489,10 @@
       </c>
     </row>
     <row r="11" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="15"/>
+      <c r="A11" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="19"/>
       <c r="C11" s="1">
         <v>5</v>
       </c>
@@ -1502,7 +1502,7 @@
       <c r="E11" s="1">
         <v>10</v>
       </c>
-      <c r="F11" s="18"/>
+      <c r="F11" s="22"/>
       <c r="G11" s="7" t="s">
         <v>25</v>
       </c>
@@ -1511,10 +1511,10 @@
       </c>
     </row>
     <row r="12" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="15" t="s">
+      <c r="A12" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="15"/>
+      <c r="B12" s="19"/>
       <c r="C12" s="1">
         <v>5</v>
       </c>
@@ -1524,7 +1524,7 @@
       <c r="E12" s="1">
         <v>10</v>
       </c>
-      <c r="F12" s="18"/>
+      <c r="F12" s="22"/>
       <c r="G12" s="7" t="s">
         <v>26</v>
       </c>
@@ -1533,10 +1533,10 @@
       </c>
     </row>
     <row r="13" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="15" t="s">
+      <c r="A13" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="15"/>
+      <c r="B13" s="19"/>
       <c r="C13" s="1">
         <v>5</v>
       </c>
@@ -1546,7 +1546,7 @@
       <c r="E13" s="1">
         <v>10</v>
       </c>
-      <c r="F13" s="18"/>
+      <c r="F13" s="22"/>
       <c r="G13" s="7" t="s">
         <v>27</v>
       </c>
@@ -1555,22 +1555,22 @@
       </c>
     </row>
     <row r="14" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="25"/>
-      <c r="B14" s="26"/>
-      <c r="C14" s="26"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="28"/>
+      <c r="A14" s="20"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="24"/>
     </row>
     <row r="15" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="17" t="s">
+      <c r="A15" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="24"/>
-      <c r="C15" s="24"/>
-      <c r="D15" s="19"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="18"/>
     </row>
     <row r="16" spans="1:8" ht="31" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
@@ -1583,7 +1583,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="23" t="s">
+      <c r="A17" s="15" t="s">
         <v>0</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -1597,7 +1597,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="23"/>
+      <c r="A18" s="15"/>
       <c r="B18" s="1" t="s">
         <v>20</v>
       </c>
@@ -1609,7 +1609,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="23"/>
+      <c r="A19" s="15"/>
       <c r="B19" s="1" t="s">
         <v>23</v>
       </c>
@@ -1621,7 +1621,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="23"/>
+      <c r="A20" s="15"/>
       <c r="B20" s="1" t="s">
         <v>24</v>
       </c>
@@ -1633,7 +1633,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A21" s="23" t="s">
+      <c r="A21" s="15" t="s">
         <v>1</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -1647,7 +1647,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A22" s="23"/>
+      <c r="A22" s="15"/>
       <c r="B22" s="1" t="s">
         <v>20</v>
       </c>
@@ -1659,7 +1659,7 @@
       </c>
     </row>
     <row r="23" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A23" s="23"/>
+      <c r="A23" s="15"/>
       <c r="B23" s="1" t="s">
         <v>23</v>
       </c>
@@ -1671,7 +1671,7 @@
       </c>
     </row>
     <row r="24" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A24" s="23"/>
+      <c r="A24" s="15"/>
       <c r="B24" s="1" t="s">
         <v>24</v>
       </c>
@@ -1732,11 +1732,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="A21:A24"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="A17:A20"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:H14"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="F1:F13"/>
@@ -1753,6 +1748,11 @@
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A21:A24"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="A17:A20"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:H14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -1875,24 +1875,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="19" t="s">
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="H1" s="16"/>
+      <c r="H1" s="25"/>
     </row>
     <row r="2" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="20"/>
+      <c r="B2" s="26"/>
       <c r="C2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1902,7 +1902,7 @@
       <c r="E2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="18"/>
+      <c r="F2" s="22"/>
       <c r="G2" s="6" t="s">
         <v>30</v>
       </c>
@@ -1911,10 +1911,10 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="15"/>
+      <c r="B3" s="19"/>
       <c r="C3" s="1">
         <v>5</v>
       </c>
@@ -1924,7 +1924,7 @@
       <c r="E3" s="3">
         <v>10</v>
       </c>
-      <c r="F3" s="18"/>
+      <c r="F3" s="22"/>
       <c r="G3" s="6" t="s">
         <v>31</v>
       </c>
@@ -1933,10 +1933,10 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="15"/>
+      <c r="B4" s="19"/>
       <c r="C4" s="1">
         <v>5</v>
       </c>
@@ -1946,7 +1946,7 @@
       <c r="E4" s="3">
         <v>10</v>
       </c>
-      <c r="F4" s="18"/>
+      <c r="F4" s="22"/>
       <c r="G4" s="6" t="s">
         <v>32</v>
       </c>
@@ -1955,10 +1955,10 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="15"/>
+      <c r="B5" s="19"/>
       <c r="C5" s="1">
         <v>5</v>
       </c>
@@ -1968,7 +1968,7 @@
       <c r="E5" s="3">
         <v>10</v>
       </c>
-      <c r="F5" s="18"/>
+      <c r="F5" s="22"/>
       <c r="G5" s="6" t="s">
         <v>33</v>
       </c>
@@ -1977,10 +1977,10 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="15"/>
+      <c r="A6" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="19"/>
       <c r="C6" s="1">
         <v>5</v>
       </c>
@@ -1990,7 +1990,7 @@
       <c r="E6" s="3">
         <v>10</v>
       </c>
-      <c r="F6" s="18"/>
+      <c r="F6" s="22"/>
       <c r="G6" s="6" t="s">
         <v>34</v>
       </c>
@@ -1999,10 +1999,10 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="15"/>
+      <c r="B7" s="19"/>
       <c r="C7" s="1">
         <v>5</v>
       </c>
@@ -2012,15 +2012,15 @@
       <c r="E7" s="3">
         <v>10</v>
       </c>
-      <c r="F7" s="18"/>
-      <c r="G7" s="21"/>
-      <c r="H7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="28"/>
     </row>
     <row r="8" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="15"/>
+      <c r="B8" s="19"/>
       <c r="C8" s="1">
         <v>5</v>
       </c>
@@ -2030,17 +2030,17 @@
       <c r="E8" s="3">
         <v>10</v>
       </c>
-      <c r="F8" s="18"/>
-      <c r="G8" s="19" t="s">
+      <c r="F8" s="22"/>
+      <c r="G8" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="H8" s="16"/>
+      <c r="H8" s="25"/>
     </row>
     <row r="9" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="15"/>
+      <c r="B9" s="19"/>
       <c r="C9" s="1">
         <v>5</v>
       </c>
@@ -2050,7 +2050,7 @@
       <c r="E9" s="3">
         <v>10</v>
       </c>
-      <c r="F9" s="18"/>
+      <c r="F9" s="22"/>
       <c r="G9" s="7" t="s">
         <v>14</v>
       </c>
@@ -2059,10 +2059,10 @@
       </c>
     </row>
     <row r="10" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="15"/>
+      <c r="B10" s="19"/>
       <c r="C10" s="1">
         <v>5</v>
       </c>
@@ -2072,7 +2072,7 @@
       <c r="E10" s="3">
         <v>10</v>
       </c>
-      <c r="F10" s="18"/>
+      <c r="F10" s="22"/>
       <c r="G10" s="7" t="s">
         <v>15</v>
       </c>
@@ -2081,10 +2081,10 @@
       </c>
     </row>
     <row r="11" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="15"/>
+      <c r="A11" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="19"/>
       <c r="C11" s="1">
         <v>5</v>
       </c>
@@ -2094,7 +2094,7 @@
       <c r="E11" s="3">
         <v>10</v>
       </c>
-      <c r="F11" s="18"/>
+      <c r="F11" s="22"/>
       <c r="G11" s="7" t="s">
         <v>25</v>
       </c>
@@ -2103,10 +2103,10 @@
       </c>
     </row>
     <row r="12" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="15" t="s">
+      <c r="A12" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="15"/>
+      <c r="B12" s="19"/>
       <c r="C12" s="1">
         <v>5</v>
       </c>
@@ -2116,7 +2116,7 @@
       <c r="E12" s="3">
         <v>10</v>
       </c>
-      <c r="F12" s="18"/>
+      <c r="F12" s="22"/>
       <c r="G12" s="7" t="s">
         <v>26</v>
       </c>
@@ -2125,10 +2125,10 @@
       </c>
     </row>
     <row r="13" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="15" t="s">
+      <c r="A13" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="15"/>
+      <c r="B13" s="19"/>
       <c r="C13" s="1">
         <v>5</v>
       </c>
@@ -2138,7 +2138,7 @@
       <c r="E13" s="3">
         <v>10</v>
       </c>
-      <c r="F13" s="18"/>
+      <c r="F13" s="22"/>
       <c r="G13" s="7" t="s">
         <v>27</v>
       </c>
@@ -2147,22 +2147,22 @@
       </c>
     </row>
     <row r="14" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="25"/>
-      <c r="B14" s="26"/>
-      <c r="C14" s="26"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="28"/>
+      <c r="A14" s="20"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="24"/>
     </row>
     <row r="15" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="17" t="s">
+      <c r="A15" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="24"/>
-      <c r="C15" s="24"/>
-      <c r="D15" s="19"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="18"/>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
@@ -2182,7 +2182,7 @@
       <c r="G16" s="4"/>
     </row>
     <row r="17" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="23" t="s">
+      <c r="A17" s="15" t="s">
         <v>0</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -2199,7 +2199,7 @@
       <c r="G17" s="4"/>
     </row>
     <row r="18" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="23"/>
+      <c r="A18" s="15"/>
       <c r="B18" s="1" t="s">
         <v>20</v>
       </c>
@@ -2214,7 +2214,7 @@
       <c r="G18" s="4"/>
     </row>
     <row r="19" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="23"/>
+      <c r="A19" s="15"/>
       <c r="B19" s="1" t="s">
         <v>23</v>
       </c>
@@ -2229,7 +2229,7 @@
       <c r="G19" s="4"/>
     </row>
     <row r="20" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="23"/>
+      <c r="A20" s="15"/>
       <c r="B20" s="1" t="s">
         <v>24</v>
       </c>
@@ -2244,7 +2244,7 @@
       <c r="G20" s="4"/>
     </row>
     <row r="21" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A21" s="23" t="s">
+      <c r="A21" s="15" t="s">
         <v>1</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -2261,7 +2261,7 @@
       <c r="G21" s="4"/>
     </row>
     <row r="22" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A22" s="23"/>
+      <c r="A22" s="15"/>
       <c r="B22" s="1" t="s">
         <v>20</v>
       </c>
@@ -2276,7 +2276,7 @@
       <c r="G22" s="4"/>
     </row>
     <row r="23" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A23" s="23"/>
+      <c r="A23" s="15"/>
       <c r="B23" s="1" t="s">
         <v>23</v>
       </c>
@@ -2291,7 +2291,7 @@
       <c r="G23" s="4"/>
     </row>
     <row r="24" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A24" s="23"/>
+      <c r="A24" s="15"/>
       <c r="B24" s="1" t="s">
         <v>24</v>
       </c>
@@ -2307,6 +2307,11 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A14:H14"/>
+    <mergeCell ref="A17:A20"/>
+    <mergeCell ref="A21:A24"/>
+    <mergeCell ref="A15:D15"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="G8:H8"/>
@@ -2323,11 +2328,6 @@
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A14:H14"/>
-    <mergeCell ref="A17:A20"/>
-    <mergeCell ref="A21:A24"/>
-    <mergeCell ref="A15:D15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2480,18 +2480,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2513,6 +2513,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3E385B-6A76-4FBB-B927-F57099B6C822}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E1C46DBC-9747-43C5-8BD2-A3AA9186CCF6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -2526,12 +2534,4 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3E385B-6A76-4FBB-B927-F57099B6C822}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>